<commit_message>
Add export PHIEU THU
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuThuTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuThuTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>RECEIPT / PHIẾU THU</t>
   </si>
@@ -32,9 +32,6 @@
     <t xml:space="preserve">Date : </t>
   </si>
   <si>
-    <t>Ngày  ………….tháng …….….năm…………</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quyển: </t>
   </si>
   <si>
@@ -42,9 +39,6 @@
   </si>
   <si>
     <t>NO/SỐ:</t>
-  </si>
-  <si>
-    <t>(chạy số tt)</t>
   </si>
   <si>
     <t>Payer/ Người nộp tiền:</t>
@@ -85,6 +79,21 @@
   <si>
     <t>308 / 18 Binh Loi St., Ward 13, Binh Thanh Dist., Ho Chi Minh City, Vietnam 
 Tel: +84 8 62581123 - Fax: +84 8 62581129 - Email: expo@aelvn.com - Website: http://www.aelvn.com</t>
+  </si>
+  <si>
+    <t>Ngày  ${day} tháng ${month} năm ${year}</t>
+  </si>
+  <si>
+    <t>${refNo}</t>
+  </si>
+  <si>
+    <t>${employee.firstName} ${employee.lastName}</t>
+  </si>
+  <si>
+    <t>${reason}</t>
+  </si>
+  <si>
+    <t>${amount}</t>
   </si>
 </sst>
 </file>
@@ -195,9 +204,6 @@
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -215,9 +221,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -234,25 +237,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,7 +619,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -626,256 +635,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
     </row>
     <row r="4" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" s="12" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+    </row>
+    <row r="6" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" s="20" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="1:10" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" s="23" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-    </row>
-    <row r="14" spans="1:10" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22" t="s">
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+    </row>
+    <row r="15" spans="1:10" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-    </row>
-    <row r="15" spans="1:10" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28" t="s">
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-    </row>
-    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
Fix download phieu thu
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuThuTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuThuTemplate.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="6120" yWindow="1635" windowWidth="17805" windowHeight="4200"/>
   </bookViews>
   <sheets>
     <sheet name="PHIEU THU " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>RECEIPT / PHIẾU THU</t>
   </si>
@@ -92,6 +93,9 @@
   </si>
   <si>
     <t>${amountVND}</t>
+  </si>
+  <si>
+    <t>${voucherNo}</t>
   </si>
 </sst>
 </file>
@@ -222,20 +226,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -243,29 +235,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,7 +616,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,56 +627,56 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="22"/>
-    <col min="4" max="4" width="10.7109375" style="22" customWidth="1"/>
-    <col min="5" max="5" width="4.5703125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="22"/>
-    <col min="10" max="10" width="11.85546875" style="22" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="25.5703125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="17"/>
+    <col min="4" max="4" width="10.7109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="17"/>
+    <col min="10" max="10" width="11.85546875" style="17" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -690,7 +694,7 @@
       </c>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" s="11" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -705,10 +709,12 @@
       <c r="H5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="6" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -720,11 +726,11 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -732,174 +738,174 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="21"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="1:10" s="11" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="23" t="s">
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+    </row>
+    <row r="15" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27" t="s">
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>